<commit_message>
created pdf library and added one item
</commit_message>
<xml_diff>
--- a/inventory/INVENTORY OF PYU INSCRIPTIONS.xlsx
+++ b/inventory/INVENTORY OF PYU INSCRIPTIONS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="497">
   <si>
     <r>
       <t>Building of a shrine by Prince R</t>
@@ -204,9 +204,6 @@
     <t>silver bowl</t>
   </si>
   <si>
-    <t>Mahlo</t>
-  </si>
-  <si>
     <t>A:?, B:?</t>
   </si>
   <si>
@@ -1082,9 +1079,6 @@
     <t>ASB 1958, pl. 16, 17.</t>
   </si>
   <si>
-    <t>Mya 1961, II, 31. — PPPB I, 155.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">ASB 1925, 18. — </t>
     </r>
@@ -2079,9 +2073,6 @@
       </rPr>
       <t xml:space="preserve"> RTI.</t>
     </r>
-  </si>
-  <si>
-    <t>San Win 1998, 2000-1, 2003. — unnumbered pages in MHRJ 11. —Tun Aung Chain 2003.</t>
   </si>
   <si>
     <r>
@@ -2378,18 +2369,12 @@
     <t>Tawadeintha (Tāvatiṁsa) pagoda in hills west of Sriksetra</t>
   </si>
   <si>
-    <t>ASI 1910-11, 93. — ASB 1911, 6, 44. — PPPB I, 158.</t>
-  </si>
-  <si>
     <t>two words</t>
   </si>
   <si>
     <t>Tawadeintha (Tāvatiṁsa) pagod, Sriksetra</t>
   </si>
   <si>
-    <t>ASB 1911, 6, 44.</t>
-  </si>
-  <si>
     <t>Found in 1935. We do not believe this inscription comprises any parts in Sanskrit, despite statements in the literature to that effect.</t>
   </si>
   <si>
@@ -2501,6 +2486,323 @@
     </r>
   </si>
   <si>
+    <t>De Beylié 1907a: 82-3. — ASI 1909-10, 120. — Blagden 1913-14: 127 (2). — PPPB I, 129.</t>
+  </si>
+  <si>
+    <t>De Beylié 1907a: 83 (n. 1). — Blagden 1913-14: 127 (6). —ASB 1916, 18 (with n. ‡). — Chen Yi-Sein 1960. — PPPB I, 67, 76 n. 38-39.</t>
+  </si>
+  <si>
+    <r>
+      <t>Blagden 1913-14: 127 (5).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — ASB 1912, 12 §37.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ASI 1926-27, pl. XXXVII (d), XXXVIII (c). — Le May 1956, fig. 4. — Mya 1961, II, pl. 1, 5, 6. — PPPB II, pl. 28-29. — Guy 2014: 66 (fig. 54), 81 (cat. 27). — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RTI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASB 1964, pl. 25. — PPPB II, pl. 51. —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RTI.</t>
+    </r>
+  </si>
+  <si>
+    <t>Blagden 1913-14: 127 (B2). — PPPB I, 126.</t>
+  </si>
+  <si>
+    <t>found in 1982</t>
+  </si>
+  <si>
+    <t>De Beylié 1907a: 89 fig. 62. — ASI 1909-10, pl. XLIX (12, 13). — Mya 1961, II, pl. 60 (gha). — PPPB II, 59 (f).</t>
+  </si>
+  <si>
+    <t>Luce refers to De Beylié 1907a, pl. V (3); 246 fig. 199. The latter is an error for 1907b: 246 fig. 199. Luce was wrong in citing these photos published by De Beylié, for De Beylié does not say that they show the obverse of the inscribed reverse copied in his (1907a) fig. 62. Comparing the other photos available, it seems obvious that de Beylié's V (3) and 62 have no connection with each other. Delhine Desoutter has shown us three other specimens of tablets made from the same mold.</t>
+  </si>
+  <si>
+    <t>Blagden 1913-14 (B1). — ASI 1911-12, 147. — ASB 1912, 7, 11. — PR, 47 (B), 50. — PPPB I, 48, 57 n. 13, 126-7. — Shafer 1943: 339. — Guy 2014: 76-7 (cat. 24).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Blagden 1913-14 (B2). — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IB IV, 354b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. — PPPB II, pl. 6 (d).</t>
+    </r>
+  </si>
+  <si>
+    <t>ASB 1964, 19-20, 59. — PPPB I, 65, 75 n. 26, 149.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASI 1926-27, 175-6. — PR, 34. — Le May 1956: 48. — PPPB I, 51, 57 n. 23, 137. — Falk 1997: 88-91. — Stargardt 2001: 498, 503-6. — Guy 2014: 80-2 (cat. 27).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nyunt Han </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 2006: 13. — Moore 2009: 111-12.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aung Thaw </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 1993: 135.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Minte mound, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hmawza</t>
+    </r>
+  </si>
+  <si>
+    <t>Khin Ba mound, Sriksetra</t>
+  </si>
+  <si>
+    <t>Aung Thaw 1972: 110, 116.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Aung Thaw 1972: 110-111. — Luce 1974: 126. — PPPB I, 176. —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> von Hinüber 1991: 25 n. 53. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">— Skilling </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1997a:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 95 n. 7.</t>
+    </r>
+  </si>
+  <si>
+    <t>ASI 1910-11, pl. XLVII (1-2). — ASI 1911-12, pl. LXVIII (1). — Finot 1913, plate. — PPPB II, pl. 98 (c).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ASI 1910-11, 89. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ASI 1911-12, 141-2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">— Finot 1912: 134-135 — Finot 1913. — PR, 35-36. — PPPB I, 61, 74 n. 4, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. — Stargardt 1995: 201.</t>
+    </r>
+  </si>
+  <si>
+    <t>ASI 1910-11, 93. — ASB 1911, 6, 41. — PPPB I, 158.</t>
+  </si>
+  <si>
+    <t>ASB 1911, 6, 41.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mya 1961, II, 31. — PPPB I, 155. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tun Aung Chain 2003: 9.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASI 1927-28, 127-8, 145. — Ray 1936: 19-20. — PR, 41-3. — PPPB I, 51, 57 n. 24, 65, 74 n. 22, 131-2. — Guy 1997: 91-2; 2014: 91-2 (cat. 41). — Tun Aung Chain 2003: 5-6.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2527,93 +2829,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>15. — Krech 2012: 153-65 (A).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Blagden 1913-14 (B). — EB I, 1, 59-68 (B). —  Shafer 1943: 320-37, 340-44, 357-63. — PR, 63-71. — PPPB I, 62-4, 74 n. 15. — Krech 2012: 153-65 (B).</t>
-    </r>
-  </si>
-  <si>
-    <t>De Beylié 1907a: 82-3. — ASI 1909-10, 120. — Blagden 1913-14: 127 (2). — PPPB I, 129.</t>
-  </si>
-  <si>
-    <t>De Beylié 1907a: 83 (n. 1). — Blagden 1913-14: 127 (6). —ASB 1916, 18 (with n. ‡). — Chen Yi-Sein 1960. — PPPB I, 67, 76 n. 38-39.</t>
-  </si>
-  <si>
-    <r>
-      <t>Blagden 1913-14: 127 (5).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> — ASB 1912, 12 §37.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ASI 1927-28, 127-8, 145. — Ray 1936: 19-20. — PR, 41-3. — PPPB I, 51, 57 n. 24, 65, 74 n. 22, 131-2. — Guy 1997: 91-2; 2014: 91-2 (cat. 41).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ASI 1926-27, pl. XXXVII (d), XXXVIII (c). — Le May 1956, fig. 4. — Mya 1961, II, pl. 1, 5, 6. — PPPB II, pl. 28-29. — Guy 2014: 66 (fig. 54), 81 (cat. 27). — </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RTI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ASB 1964, pl. 25. — PPPB II, pl. 51. —</t>
+      <t>15. — Tun Aung Chain 2003: 7-8. — Krech 2012: 153-65 (A).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Blagden 1913-14 (B). — EB I, 1, 59-68 (B). —  Shafer 1943: 320-37, 340-44, 357-63. — PR, 63-71. — PPPB I, 62-4, 74 n. 15. — Tun Aung Chain 2003: 7-8. — Krech 2012: 153-65 (B).</t>
+    </r>
+  </si>
+  <si>
+    <t>Mahlo 2012: 167 (app. 27.1).</t>
+  </si>
+  <si>
+    <t>Mahlo 2012: 167 (app. 27.2).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">San Win 1998, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2000-1, 2003. —</t>
     </r>
     <r>
       <rPr>
@@ -2623,219 +2870,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> RTI.</t>
-    </r>
-  </si>
-  <si>
-    <t>Blagden 1913-14: 127 (B2). — PPPB I, 126.</t>
-  </si>
-  <si>
-    <t>found in 1982</t>
-  </si>
-  <si>
-    <t>De Beylié 1907a: 89 fig. 62. — ASI 1909-10, pl. XLIX (12, 13). — Mya 1961, II, pl. 60 (gha). — PPPB II, 59 (f).</t>
-  </si>
-  <si>
-    <t>Luce refers to De Beylié 1907a, pl. V (3); 246 fig. 199. The latter is an error for 1907b: 246 fig. 199. Luce was wrong in citing these photos published by De Beylié, for De Beylié does not say that they show the obverse of the inscribed reverse copied in his (1907a) fig. 62. Comparing the other photos available, it seems obvious that de Beylié's V (3) and 62 have no connection with each other. Delhine Desoutter has shown us three other specimens of tablets made from the same mold.</t>
-  </si>
-  <si>
-    <t>Blagden 1913-14 (B1). — ASI 1911-12, 147. — ASB 1912, 7, 11. — PR, 47 (B), 50. — PPPB I, 48, 57 n. 13, 126-7. — Shafer 1943: 339. — Guy 2014: 76-7 (cat. 24).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Blagden 1913-14 (B2). — </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IB IV, 354b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. — PPPB II, pl. 6 (d).</t>
-    </r>
-  </si>
-  <si>
-    <t>ASB 1964, 19-20, 59. — PPPB I, 65, 75 n. 26, 149.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ASI 1926-27, 175-6. — PR, 34. — Le May 1956: 48. — PPPB I, 51, 57 n. 23, 137. — Falk 1997: 88-91. — Stargardt 2001: 498, 503-6. — Guy 2014: 80-2 (cat. 27).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nyunt Han </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. 2006: 13. — Moore 2009: 111-12.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Aung Thaw </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. 1993: 135.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Minte mound, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Hmawza</t>
-    </r>
-  </si>
-  <si>
-    <t>Khin Ba mound, Sriksetra</t>
-  </si>
-  <si>
-    <t>Aung Thaw 1972: 110, 116.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Aung Thaw 1972: 110-111. — Luce 1974: 126. — PPPB I, 176. —</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> von Hinüber 1991: 25 n. 53. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">— Skilling </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1997a:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 95 n. 7.</t>
-    </r>
-  </si>
-  <si>
-    <t>ASI 1910-11, pl. XLVII (1-2). — ASI 1911-12, pl. LXVIII (1). — Finot 1913, plate. — PPPB II, pl. 98 (c).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ASI 1910-11, 89. — </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ASI 1911-12, 141-2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">— Finot 1912: 134-135 — Finot 1913. — PR, 35-36. — PPPB I, 61, 74 n. 4, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>XX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. — Stargardt 1995: 201.</t>
+      <t xml:space="preserve"> unnumbered pages in MHRJ 11. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>—Tun Aung Chain 2003: 1-4.</t>
     </r>
   </si>
 </sst>
@@ -3081,7 +3125,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="229">
+  <cellStyleXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3311,8 +3355,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3477,6 +3523,9 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3498,11 +3547,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="229">
+  <cellStyles count="231">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3617,6 +3666,7 @@
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3731,6 +3781,7 @@
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4023,10 +4074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K125"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4043,7 +4094,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="4"/>
@@ -4051,10 +4102,10 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="62" t="s">
-        <v>375</v>
-      </c>
-      <c r="C2" s="62"/>
+      <c r="B2" s="63" t="s">
+        <v>373</v>
+      </c>
+      <c r="C2" s="63"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
         <v>1</v>
@@ -4064,34 +4115,34 @@
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="65" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="68" t="s">
+      <c r="D3" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="63" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="64" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4099,47 +4150,47 @@
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:11" ht="59">
       <c r="A5" s="9">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C5" s="11">
         <v>2</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>190</v>
-      </c>
       <c r="H5" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="K5" s="10"/>
     </row>
@@ -4148,29 +4199,29 @@
         <v>2</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="19" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>20</v>
@@ -4181,34 +4232,34 @@
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="56">
@@ -4216,31 +4267,31 @@
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K8" s="10"/>
     </row>
@@ -4249,31 +4300,31 @@
         <v>5</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>8</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="K9" s="10"/>
     </row>
@@ -4282,104 +4333,104 @@
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="70">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="84">
       <c r="A11" s="9">
         <v>7</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>472</v>
+        <v>492</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="56">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="70">
       <c r="A12" s="9">
         <v>8</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G12" s="46" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>473</v>
+        <v>493</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="42">
@@ -4387,27 +4438,27 @@
         <v>9</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="K13" s="10"/>
     </row>
@@ -4416,31 +4467,31 @@
         <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H14" s="26" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="K14" s="10"/>
     </row>
@@ -4449,34 +4500,34 @@
         <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H15" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="42">
@@ -4484,29 +4535,29 @@
         <v>12</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>144</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>25</v>
@@ -4517,7 +4568,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>29</v>
@@ -4528,16 +4579,16 @@
         <v>3</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="H17" s="69" t="s">
-        <v>456</v>
+        <v>220</v>
+      </c>
+      <c r="H17" s="62" t="s">
+        <v>453</v>
       </c>
       <c r="I17" s="46" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="K17" s="46"/>
     </row>
@@ -4546,7 +4597,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>19</v>
@@ -4554,22 +4605,22 @@
       <c r="D18" s="30"/>
       <c r="E18" s="47"/>
       <c r="F18" s="46" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H18" s="45" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I18" s="46" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="K18" s="46" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="42">
@@ -4577,60 +4628,60 @@
         <v>15</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H19" s="46"/>
       <c r="I19" s="46" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>461</v>
+        <v>488</v>
       </c>
       <c r="K19" s="45" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="56">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="70">
       <c r="A20" s="21">
         <v>16</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>193</v>
-      </c>
       <c r="D20" s="28" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="K20" s="13"/>
     </row>
@@ -4639,32 +4690,32 @@
         <v>17</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="20">
         <v>8</v>
       </c>
       <c r="D21" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="G21" s="24" t="s">
         <v>194</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>400</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>195</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="22" customFormat="1" ht="56">
@@ -4672,30 +4723,30 @@
         <v>18</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="28">
@@ -4703,30 +4754,30 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C23" s="20">
         <v>3</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J23" s="22"/>
       <c r="K23" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="22" customFormat="1" ht="70">
@@ -4734,29 +4785,29 @@
         <v>20</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C24" s="20">
         <v>5</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>439</v>
+        <v>496</v>
       </c>
       <c r="K24" s="13"/>
     </row>
@@ -4765,30 +4816,30 @@
         <v>21</v>
       </c>
       <c r="B25" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>81</v>
-      </c>
       <c r="G25" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="6" customFormat="1" ht="84">
@@ -4796,32 +4847,32 @@
         <v>22</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="13" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="112">
@@ -4829,30 +4880,30 @@
         <v>23</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G27" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="70">
@@ -4860,29 +4911,29 @@
         <v>24</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="19" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="K28" s="13"/>
     </row>
@@ -4891,32 +4942,32 @@
         <v>25</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="28">
@@ -4924,32 +4975,32 @@
         <v>26</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="19" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="28">
@@ -4957,29 +5008,29 @@
         <v>27</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="G31" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>197</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="13" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="K31" s="13"/>
     </row>
@@ -4988,30 +5039,30 @@
         <v>28</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="28" t="s">
-        <v>102</v>
-      </c>
       <c r="D32" s="28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="28">
@@ -5019,30 +5070,30 @@
         <v>29</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="25" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="13" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="28">
@@ -5050,30 +5101,30 @@
         <v>30</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H34" s="24"/>
       <c r="I34" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="28">
@@ -5081,26 +5132,26 @@
         <v>31</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
@@ -5110,32 +5161,32 @@
         <v>32</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>151</v>
-      </c>
       <c r="E36" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="28">
@@ -5143,27 +5194,27 @@
         <v>33</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E37" s="19"/>
       <c r="F37" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K37" s="13"/>
     </row>
@@ -5172,32 +5223,32 @@
         <v>34</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J38" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="K38" s="12" t="s">
         <v>335</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="56">
@@ -5205,29 +5256,29 @@
         <v>35</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="E39" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="G39" s="12" t="s">
         <v>200</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K39" s="13"/>
     </row>
@@ -5236,32 +5287,32 @@
         <v>36</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="84">
@@ -5269,32 +5320,32 @@
         <v>37</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="48" t="s">
+        <v>348</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>352</v>
-      </c>
       <c r="G41" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="22" customFormat="1" ht="28">
@@ -5308,23 +5359,23 @@
         <v>19</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K42" s="13"/>
     </row>
@@ -5333,30 +5384,30 @@
         <v>39</v>
       </c>
       <c r="B43" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43" s="29" t="s">
         <v>153</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>408</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>154</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J43" s="13"/>
       <c r="K43" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="56">
@@ -5364,32 +5415,32 @@
         <v>40</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="19" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="28">
@@ -5397,29 +5448,29 @@
         <v>41</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="23" t="s">
-        <v>105</v>
-      </c>
       <c r="G45" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K45" s="13"/>
     </row>
@@ -5428,29 +5479,29 @@
         <v>42</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K46" s="13"/>
     </row>
@@ -5459,25 +5510,25 @@
         <v>43</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="19" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K47" s="13"/>
     </row>
@@ -5486,32 +5537,32 @@
         <v>44</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="19" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="42">
@@ -5519,29 +5570,29 @@
         <v>45</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D49" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="G49" s="12" t="s">
         <v>371</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>373</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K49" s="13"/>
     </row>
@@ -5550,27 +5601,27 @@
         <v>46</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D50" s="28"/>
       <c r="E50" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K50" s="13"/>
     </row>
@@ -5586,17 +5637,17 @@
       </c>
       <c r="D51" s="28"/>
       <c r="E51" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H51" s="18"/>
       <c r="I51" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="18"/>
@@ -5613,17 +5664,17 @@
       </c>
       <c r="D52" s="28"/>
       <c r="E52" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H52" s="18"/>
       <c r="I52" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="18"/>
@@ -5633,27 +5684,27 @@
         <v>49</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K53" s="19"/>
     </row>
@@ -5662,27 +5713,27 @@
         <v>50</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C54" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G54" s="12"/>
       <c r="H54" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I54" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="J54" s="12" t="s">
         <v>228</v>
-      </c>
-      <c r="J54" s="12" t="s">
-        <v>229</v>
       </c>
       <c r="K54" s="12"/>
     </row>
@@ -5691,26 +5742,26 @@
         <v>51</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H55" s="19"/>
       <c r="I55" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
@@ -5720,29 +5771,29 @@
         <v>52</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H56" s="19"/>
       <c r="I56" s="23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K56" s="19"/>
     </row>
@@ -5757,23 +5808,23 @@
         <v>19</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H57" s="19"/>
       <c r="I57" s="23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K57" s="19"/>
     </row>
@@ -5788,23 +5839,23 @@
         <v>19</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H58" s="19"/>
       <c r="I58" s="23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K58" s="19"/>
     </row>
@@ -5813,23 +5864,23 @@
         <v>55</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="20"/>
       <c r="D59" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E59" s="23"/>
       <c r="F59" s="19"/>
       <c r="G59" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H59" s="19"/>
       <c r="I59" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J59" s="23" t="s">
         <v>95</v>
-      </c>
-      <c r="J59" s="23" t="s">
-        <v>96</v>
       </c>
       <c r="K59" s="19"/>
     </row>
@@ -5838,20 +5889,20 @@
         <v>56</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E60" s="23"/>
       <c r="F60" s="19"/>
       <c r="G60" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
@@ -5861,20 +5912,20 @@
         <v>57</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E61" s="23"/>
       <c r="F61" s="19"/>
       <c r="G61" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H61" s="19"/>
       <c r="I61" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
@@ -5884,29 +5935,29 @@
         <v>58</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C62" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K62" s="23"/>
     </row>
@@ -5915,27 +5966,27 @@
         <v>59</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="G63" s="23" t="s">
         <v>108</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="G63" s="23" t="s">
-        <v>109</v>
       </c>
       <c r="H63" s="23"/>
       <c r="I63" s="23" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J63" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K63" s="19"/>
     </row>
@@ -5944,24 +5995,24 @@
         <v>60</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H64" s="23"/>
       <c r="I64" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J64" s="19"/>
       <c r="K64" s="19"/>
@@ -5977,24 +6028,24 @@
         <v>19</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G65" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H65" s="23"/>
       <c r="I65" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J65" s="19"/>
       <c r="K65" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="22" customFormat="1">
@@ -6002,22 +6053,22 @@
         <v>62</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C66" s="28"/>
       <c r="D66" s="28"/>
       <c r="E66" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
@@ -6027,31 +6078,31 @@
         <v>63</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D67" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="E67" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="F67" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="J67" s="12" t="s">
         <v>383</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>382</v>
-      </c>
-      <c r="H67" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="I67" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="J67" s="12" t="s">
-        <v>385</v>
       </c>
       <c r="K67" s="12"/>
     </row>
@@ -6060,24 +6111,24 @@
         <v>64</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C68" s="28" t="s">
         <v>27</v>
       </c>
       <c r="D68" s="28"/>
       <c r="E68" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
       <c r="K68" s="12" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="22" customFormat="1" ht="42">
@@ -6085,29 +6136,29 @@
         <v>65</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C69" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D69" s="28"/>
       <c r="E69" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G69" s="12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H69" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="J69" s="12" t="s">
         <v>397</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="J69" s="12" t="s">
-        <v>399</v>
       </c>
       <c r="K69" s="12"/>
     </row>
@@ -6116,29 +6167,29 @@
         <v>66</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" s="58" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D70" s="58"/>
       <c r="E70" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G70" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H70" s="59" t="s">
+        <v>391</v>
+      </c>
+      <c r="I70" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="J70" s="24" t="s">
         <v>393</v>
-      </c>
-      <c r="I70" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="J70" s="24" t="s">
-        <v>395</v>
       </c>
       <c r="K70" s="59"/>
     </row>
@@ -6150,447 +6201,438 @@
         <v>33</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J71" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K71" s="18"/>
     </row>
     <row r="72" spans="1:11" s="49" customFormat="1">
-      <c r="A72" s="33"/>
+      <c r="A72" s="70">
+        <v>68</v>
+      </c>
       <c r="B72" s="36" t="s">
         <v>33</v>
       </c>
       <c r="C72" s="35"/>
       <c r="D72" s="35"/>
-      <c r="E72" s="36"/>
+      <c r="E72" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="F72" s="36"/>
       <c r="G72" s="36"/>
       <c r="H72" s="36"/>
       <c r="I72" s="36"/>
       <c r="J72" s="36" t="s">
-        <v>53</v>
+        <v>494</v>
       </c>
       <c r="K72" s="36"/>
     </row>
     <row r="73" spans="1:11" s="49" customFormat="1">
-      <c r="A73" s="33"/>
+      <c r="A73" s="70">
+        <v>69</v>
+      </c>
       <c r="B73" s="36" t="s">
         <v>33</v>
       </c>
       <c r="C73" s="35"/>
       <c r="D73" s="35"/>
-      <c r="E73" s="36"/>
+      <c r="E73" s="36" t="s">
+        <v>55</v>
+      </c>
       <c r="F73" s="36"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
       <c r="I73" s="36"/>
       <c r="J73" s="36" t="s">
-        <v>53</v>
+        <v>495</v>
       </c>
       <c r="K73" s="36"/>
     </row>
     <row r="74" spans="1:11" s="22" customFormat="1" ht="28">
-      <c r="A74" s="41"/>
+      <c r="A74" s="70">
+        <v>70</v>
+      </c>
       <c r="B74" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C74" s="43"/>
+        <v>280</v>
+      </c>
+      <c r="C74" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="D74" s="43"/>
       <c r="E74" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F74" s="42"/>
-      <c r="G74" s="42" t="s">
-        <v>318</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F74" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="G74" s="34"/>
       <c r="H74" s="42"/>
-      <c r="I74" s="61" t="s">
-        <v>392</v>
+      <c r="I74" s="42" t="s">
+        <v>311</v>
       </c>
       <c r="J74" s="42" t="s">
-        <v>396</v>
+        <v>490</v>
       </c>
       <c r="K74" s="42"/>
     </row>
-    <row r="75" spans="1:11" s="22" customFormat="1">
+    <row r="75" spans="1:11" s="22" customFormat="1" ht="28">
       <c r="A75" s="41"/>
       <c r="B75" s="42" t="s">
-        <v>282</v>
-      </c>
-      <c r="C75" s="43" t="s">
-        <v>30</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C75" s="43"/>
       <c r="D75" s="43"/>
       <c r="E75" s="42" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F75" s="42"/>
       <c r="G75" s="42" t="s">
-        <v>109</v>
+        <v>316</v>
       </c>
       <c r="H75" s="42"/>
-      <c r="I75" s="42"/>
+      <c r="I75" s="61" t="s">
+        <v>390</v>
+      </c>
       <c r="J75" s="42" t="s">
-        <v>298</v>
-      </c>
-      <c r="K75" s="42" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="22" customFormat="1" ht="28">
+        <v>394</v>
+      </c>
+      <c r="K75" s="42"/>
+    </row>
+    <row r="76" spans="1:11" s="22" customFormat="1">
       <c r="A76" s="41"/>
       <c r="B76" s="42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D76" s="43"/>
       <c r="E76" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F76" s="42" t="s">
+      <c r="F76" s="42"/>
+      <c r="G76" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
+      <c r="J76" s="42" t="s">
         <v>296</v>
       </c>
-      <c r="G76" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="H76" s="36"/>
-      <c r="I76" s="42" t="s">
-        <v>295</v>
-      </c>
-      <c r="J76" s="42" t="s">
-        <v>294</v>
-      </c>
-      <c r="K76" s="36"/>
-    </row>
-    <row r="77" spans="1:11" s="22" customFormat="1" ht="56">
+      <c r="K76" s="42" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="22" customFormat="1" ht="28">
       <c r="A77" s="41"/>
       <c r="B77" s="42" t="s">
-        <v>107</v>
+        <v>280</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D77" s="43"/>
       <c r="E77" s="42" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F77" s="42" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="G77" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="H77" s="42"/>
+        <v>108</v>
+      </c>
+      <c r="H77" s="36"/>
       <c r="I77" s="42" t="s">
-        <v>344</v>
+        <v>293</v>
       </c>
       <c r="J77" s="42" t="s">
-        <v>346</v>
-      </c>
-      <c r="K77" s="42" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" s="22" customFormat="1" ht="28">
+        <v>292</v>
+      </c>
+      <c r="K77" s="36"/>
+    </row>
+    <row r="78" spans="1:11" s="22" customFormat="1" ht="56">
       <c r="A78" s="41"/>
       <c r="B78" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D78" s="43"/>
-      <c r="E78" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F78" s="42"/>
-      <c r="G78" s="34"/>
+      <c r="E78" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="F78" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="G78" s="42" t="s">
+        <v>108</v>
+      </c>
       <c r="H78" s="42"/>
       <c r="I78" s="42" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="J78" s="42" t="s">
-        <v>320</v>
-      </c>
-      <c r="K78" s="42"/>
-    </row>
-    <row r="79" spans="1:11" s="22" customFormat="1">
+        <v>344</v>
+      </c>
+      <c r="K78" s="42" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="22" customFormat="1" ht="28">
       <c r="A79" s="41"/>
       <c r="B79" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C79" s="43"/>
+        <v>106</v>
+      </c>
+      <c r="C79" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="D79" s="43"/>
-      <c r="E79" s="34"/>
+      <c r="E79" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="F79" s="42"/>
       <c r="G79" s="34"/>
       <c r="H79" s="42"/>
-      <c r="I79" s="34" t="s">
-        <v>292</v>
-      </c>
-      <c r="J79" s="34" t="s">
-        <v>278</v>
+      <c r="I79" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="J79" s="42" t="s">
+        <v>318</v>
       </c>
       <c r="K79" s="42"/>
     </row>
-    <row r="80" spans="1:11" s="22" customFormat="1" ht="112">
-      <c r="A80" s="54"/>
-      <c r="B80" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C80" s="55" t="s">
+    <row r="80" spans="1:11" s="22" customFormat="1">
+      <c r="A80" s="41"/>
+      <c r="B80" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="42"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="42"/>
+      <c r="I80" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="J80" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="K80" s="42"/>
+    </row>
+    <row r="81" spans="1:11" s="22" customFormat="1" ht="112">
+      <c r="A81" s="54"/>
+      <c r="B81" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D80" s="55"/>
-      <c r="E80" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="F80" s="42" t="s">
-        <v>274</v>
-      </c>
-      <c r="G80" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="H80" s="36"/>
-      <c r="I80" s="42" t="s">
+      <c r="D81" s="55"/>
+      <c r="E81" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="J80" s="42" t="s">
+      <c r="G81" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="H81" s="36"/>
+      <c r="I81" s="42" t="s">
         <v>272</v>
       </c>
-      <c r="K80" s="36" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" s="22" customFormat="1" ht="28">
-      <c r="A81" s="41"/>
-      <c r="B81" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C81" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D81" s="43"/>
-      <c r="E81" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F81" s="42"/>
-      <c r="G81" s="34"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="42" t="s">
-        <v>285</v>
-      </c>
       <c r="J81" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="K81" s="42"/>
-    </row>
-    <row r="82" spans="1:11" s="22" customFormat="1">
+        <v>271</v>
+      </c>
+      <c r="K81" s="36" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" s="22" customFormat="1" ht="28">
       <c r="A82" s="41"/>
       <c r="B82" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C82" s="43" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D82" s="43"/>
       <c r="E82" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F82" s="42"/>
       <c r="G82" s="34"/>
       <c r="H82" s="42"/>
       <c r="I82" s="42" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="J82" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="K82" s="34" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" s="22" customFormat="1" ht="28">
+        <v>284</v>
+      </c>
+      <c r="K82" s="42"/>
+    </row>
+    <row r="83" spans="1:11" s="22" customFormat="1">
       <c r="A83" s="41"/>
       <c r="B83" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C83" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D83" s="43"/>
       <c r="E83" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F83" s="42" t="s">
-        <v>277</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F83" s="42"/>
       <c r="G83" s="34"/>
       <c r="H83" s="42"/>
       <c r="I83" s="42" t="s">
-        <v>275</v>
+        <v>309</v>
       </c>
       <c r="J83" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="K83" s="42"/>
-    </row>
-    <row r="84" spans="1:11" s="22" customFormat="1">
+        <v>284</v>
+      </c>
+      <c r="K83" s="34" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="22" customFormat="1" ht="28">
       <c r="A84" s="41"/>
       <c r="B84" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C84" s="43"/>
+        <v>106</v>
+      </c>
+      <c r="C84" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="D84" s="43"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="42"/>
+      <c r="E84" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F84" s="42" t="s">
+        <v>276</v>
+      </c>
       <c r="G84" s="34"/>
       <c r="H84" s="42"/>
-      <c r="I84" s="34" t="s">
-        <v>279</v>
-      </c>
-      <c r="J84" s="34" t="s">
-        <v>278</v>
+      <c r="I84" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="J84" s="42" t="s">
+        <v>275</v>
       </c>
       <c r="K84" s="42"/>
     </row>
-    <row r="85" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="85" spans="1:11" s="22" customFormat="1">
       <c r="A85" s="41"/>
       <c r="B85" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" s="43" t="s">
-        <v>19</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C85" s="43"/>
       <c r="D85" s="43"/>
       <c r="E85" s="34"/>
       <c r="F85" s="42"/>
       <c r="G85" s="34"/>
       <c r="H85" s="42"/>
-      <c r="I85" s="42" t="s">
-        <v>312</v>
+      <c r="I85" s="34" t="s">
+        <v>278</v>
       </c>
       <c r="J85" s="34" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K85" s="42"/>
     </row>
     <row r="86" spans="1:11" s="22" customFormat="1" ht="28">
       <c r="A86" s="41"/>
       <c r="B86" s="42" t="s">
-        <v>282</v>
+        <v>106</v>
       </c>
       <c r="C86" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D86" s="43"/>
-      <c r="E86" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F86" s="42" t="s">
-        <v>283</v>
-      </c>
+      <c r="E86" s="34"/>
+      <c r="F86" s="42"/>
       <c r="G86" s="34"/>
       <c r="H86" s="42"/>
       <c r="I86" s="42" t="s">
-        <v>313</v>
-      </c>
-      <c r="J86" s="42" t="s">
-        <v>280</v>
+        <v>310</v>
+      </c>
+      <c r="J86" s="34" t="s">
+        <v>279</v>
       </c>
       <c r="K86" s="42"/>
     </row>
-    <row r="87" spans="1:11" s="22" customFormat="1">
-      <c r="A87" s="41"/>
-      <c r="B87" s="42" t="s">
-        <v>282</v>
-      </c>
-      <c r="C87" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D87" s="43"/>
-      <c r="E87" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F87" s="42" t="s">
-        <v>283</v>
-      </c>
-      <c r="G87" s="34"/>
-      <c r="H87" s="42"/>
-      <c r="I87" s="42" t="s">
-        <v>314</v>
-      </c>
-      <c r="J87" s="42" t="s">
-        <v>284</v>
-      </c>
-      <c r="K87" s="42"/>
-    </row>
-    <row r="88" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="88" spans="1:11" s="22" customFormat="1">
       <c r="A88" s="41"/>
       <c r="B88" s="42" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C88" s="43" t="s">
-        <v>462</v>
+        <v>19</v>
       </c>
       <c r="D88" s="43"/>
       <c r="E88" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F88" s="42" t="s">
-        <v>463</v>
+        <v>281</v>
       </c>
       <c r="G88" s="34"/>
       <c r="H88" s="42"/>
-      <c r="I88" s="42"/>
+      <c r="I88" s="42" t="s">
+        <v>312</v>
+      </c>
       <c r="J88" s="42" t="s">
-        <v>464</v>
+        <v>282</v>
       </c>
       <c r="K88" s="42"/>
     </row>
-    <row r="89" spans="1:11" s="22" customFormat="1">
-      <c r="A89" s="33"/>
-      <c r="B89" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C89" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D89" s="35"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="H89" s="36"/>
-      <c r="I89" s="36"/>
-      <c r="J89" s="36"/>
-      <c r="K89" s="36"/>
+    <row r="89" spans="1:11" s="22" customFormat="1" ht="28">
+      <c r="A89" s="41"/>
+      <c r="B89" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="C89" s="43" t="s">
+        <v>458</v>
+      </c>
+      <c r="D89" s="43"/>
+      <c r="E89" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F89" s="42" t="s">
+        <v>459</v>
+      </c>
+      <c r="G89" s="34"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="42"/>
+      <c r="J89" s="42" t="s">
+        <v>489</v>
+      </c>
+      <c r="K89" s="42"/>
     </row>
     <row r="90" spans="1:11" s="22" customFormat="1">
       <c r="A90" s="33"/>
       <c r="B90" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C90" s="35" t="s">
         <v>30</v>
@@ -6606,64 +6648,62 @@
       <c r="J90" s="36"/>
       <c r="K90" s="36"/>
     </row>
-    <row r="91" spans="1:11" ht="42">
+    <row r="91" spans="1:11" s="22" customFormat="1">
       <c r="A91" s="33"/>
       <c r="B91" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C91" s="35"/>
+        <v>106</v>
+      </c>
+      <c r="C91" s="35" t="s">
+        <v>30</v>
+      </c>
       <c r="D91" s="35"/>
       <c r="E91" s="36"/>
       <c r="F91" s="36"/>
-      <c r="G91" s="36"/>
+      <c r="G91" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="H91" s="36"/>
-      <c r="I91" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="J91" s="36" t="s">
-        <v>261</v>
-      </c>
+      <c r="I91" s="36"/>
+      <c r="J91" s="36"/>
       <c r="K91" s="36"/>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" ht="42">
       <c r="A92" s="33"/>
-      <c r="B92" s="34"/>
+      <c r="B92" s="34" t="s">
+        <v>32</v>
+      </c>
       <c r="C92" s="35"/>
       <c r="D92" s="35"/>
       <c r="E92" s="36"/>
-      <c r="F92" s="36" t="s">
-        <v>412</v>
-      </c>
+      <c r="F92" s="36"/>
       <c r="G92" s="36"/>
       <c r="H92" s="36"/>
-      <c r="I92" s="36"/>
+      <c r="I92" s="36" t="s">
+        <v>261</v>
+      </c>
       <c r="J92" s="36" t="s">
-        <v>413</v>
+        <v>260</v>
       </c>
       <c r="K92" s="36"/>
     </row>
-    <row r="93" spans="1:11" ht="28">
-      <c r="A93" s="41"/>
-      <c r="B93" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="C93" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" s="43"/>
-      <c r="E93" s="34"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="42" t="s">
-        <v>366</v>
-      </c>
-      <c r="H93" s="42"/>
-      <c r="I93" s="42"/>
-      <c r="J93" s="42"/>
-      <c r="K93" s="42" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" s="50" customFormat="1" ht="98">
+    <row r="93" spans="1:11">
+      <c r="A93" s="33"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="35"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="36" t="s">
+        <v>411</v>
+      </c>
+      <c r="K93" s="36"/>
+    </row>
+    <row r="94" spans="1:11" ht="28">
       <c r="A94" s="41"/>
       <c r="B94" s="42" t="s">
         <v>52</v>
@@ -6672,85 +6712,83 @@
         <v>19</v>
       </c>
       <c r="D94" s="43"/>
-      <c r="E94" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F94" s="42" t="s">
-        <v>55</v>
-      </c>
+      <c r="E94" s="34"/>
+      <c r="F94" s="42"/>
       <c r="G94" s="42" t="s">
-        <v>220</v>
+        <v>364</v>
       </c>
       <c r="H94" s="42"/>
-      <c r="I94" s="34" t="s">
-        <v>218</v>
-      </c>
+      <c r="I94" s="42"/>
       <c r="J94" s="42"/>
       <c r="K94" s="42" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" s="49" customFormat="1">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" s="50" customFormat="1" ht="98">
       <c r="A95" s="41"/>
       <c r="B95" s="42" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C95" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D95" s="43"/>
       <c r="E95" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F95" s="42"/>
+        <v>55</v>
+      </c>
+      <c r="F95" s="42" t="s">
+        <v>54</v>
+      </c>
       <c r="G95" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H95" s="42"/>
-      <c r="I95" s="42"/>
-      <c r="J95" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="K95" s="42"/>
-    </row>
-    <row r="96" spans="1:11" s="50" customFormat="1">
+      <c r="I95" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="J95" s="42"/>
+      <c r="K95" s="42" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" s="49" customFormat="1">
       <c r="A96" s="41"/>
       <c r="B96" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C96" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D96" s="43"/>
       <c r="E96" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F96" s="42"/>
       <c r="G96" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H96" s="42"/>
       <c r="I96" s="42"/>
       <c r="J96" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K96" s="42"/>
     </row>
     <row r="97" spans="1:11" s="50" customFormat="1">
       <c r="A97" s="41"/>
       <c r="B97" s="42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C97" s="43" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="D97" s="43"/>
       <c r="E97" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F97" s="42"/>
       <c r="G97" s="42" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
       <c r="H97" s="42"/>
       <c r="I97" s="42"/>
@@ -6762,244 +6800,254 @@
     <row r="98" spans="1:11" s="50" customFormat="1">
       <c r="A98" s="41"/>
       <c r="B98" s="42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C98" s="43" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="D98" s="43"/>
       <c r="E98" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F98" s="42"/>
       <c r="G98" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H98" s="42"/>
       <c r="I98" s="42"/>
       <c r="J98" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="K98" s="42" t="s">
         <v>67</v>
       </c>
+      <c r="K98" s="42"/>
     </row>
     <row r="99" spans="1:11" s="50" customFormat="1">
       <c r="A99" s="41"/>
       <c r="B99" s="42" t="s">
-        <v>234</v>
+        <v>65</v>
       </c>
       <c r="C99" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D99" s="43"/>
-      <c r="E99" s="34" t="s">
-        <v>60</v>
+      <c r="E99" s="42" t="s">
+        <v>55</v>
       </c>
       <c r="F99" s="42"/>
       <c r="G99" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="H99" s="42" t="s">
-        <v>233</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="H99" s="42"/>
       <c r="I99" s="42"/>
-      <c r="J99" s="42"/>
+      <c r="J99" s="42" t="s">
+        <v>67</v>
+      </c>
       <c r="K99" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" s="50" customFormat="1" ht="28">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" s="50" customFormat="1">
       <c r="A100" s="41"/>
       <c r="B100" s="42" t="s">
-        <v>73</v>
+        <v>233</v>
       </c>
       <c r="C100" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D100" s="43"/>
-      <c r="E100" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="F100" s="42" t="s">
-        <v>76</v>
-      </c>
+      <c r="E100" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100" s="42"/>
       <c r="G100" s="42" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="H100" s="42" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="I100" s="42"/>
-      <c r="J100" s="42" t="s">
-        <v>75</v>
-      </c>
+      <c r="J100" s="42"/>
       <c r="K100" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A101" s="41"/>
       <c r="B101" s="42" t="s">
-        <v>236</v>
+        <v>72</v>
       </c>
       <c r="C101" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D101" s="43"/>
       <c r="E101" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="F101" s="42"/>
+        <v>107</v>
+      </c>
+      <c r="F101" s="42" t="s">
+        <v>75</v>
+      </c>
       <c r="G101" s="42" t="s">
-        <v>232</v>
+        <v>176</v>
       </c>
       <c r="H101" s="42" t="s">
-        <v>235</v>
+        <v>182</v>
       </c>
       <c r="I101" s="42"/>
       <c r="J101" s="42" t="s">
-        <v>418</v>
-      </c>
-      <c r="K101" s="42"/>
+        <v>74</v>
+      </c>
+      <c r="K101" s="42" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="102" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A102" s="41"/>
       <c r="B102" s="42" t="s">
-        <v>329</v>
+        <v>235</v>
       </c>
       <c r="C102" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D102" s="43"/>
       <c r="E102" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F102" s="42"/>
       <c r="G102" s="42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H102" s="42" t="s">
-        <v>330</v>
+        <v>234</v>
       </c>
       <c r="I102" s="42"/>
       <c r="J102" s="42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K102" s="42"/>
     </row>
     <row r="103" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A103" s="41"/>
       <c r="B103" s="42" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C103" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D103" s="43"/>
       <c r="E103" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F103" s="42"/>
       <c r="G103" s="42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H103" s="42" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I103" s="42"/>
       <c r="J103" s="42" t="s">
-        <v>416</v>
-      </c>
-      <c r="K103" s="42" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" s="50" customFormat="1" ht="182">
+        <v>415</v>
+      </c>
+      <c r="K103" s="42"/>
+    </row>
+    <row r="104" spans="1:11" s="50" customFormat="1" ht="28">
       <c r="A104" s="41"/>
       <c r="B104" s="42" t="s">
-        <v>184</v>
+        <v>326</v>
       </c>
       <c r="C104" s="43" t="s">
         <v>19</v>
       </c>
       <c r="D104" s="43"/>
       <c r="E104" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F104" s="42"/>
       <c r="G104" s="42" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="H104" s="42" t="s">
-        <v>186</v>
-      </c>
-      <c r="I104" s="42" t="s">
-        <v>378</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="I104" s="42"/>
       <c r="J104" s="42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K104" s="42" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" s="50" customFormat="1">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" s="50" customFormat="1" ht="182">
       <c r="A105" s="41"/>
-      <c r="B105" s="42"/>
-      <c r="C105" s="43"/>
+      <c r="B105" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="C105" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="D105" s="43"/>
-      <c r="E105" s="42"/>
+      <c r="E105" s="42" t="s">
+        <v>107</v>
+      </c>
       <c r="F105" s="42"/>
       <c r="G105" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="H105" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="I105" s="42" t="s">
+        <v>376</v>
+      </c>
+      <c r="J105" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="K105" s="42" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" s="50" customFormat="1">
+      <c r="A106" s="41"/>
+      <c r="B106" s="42"/>
+      <c r="C106" s="43"/>
+      <c r="D106" s="43"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="H106" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="I106" s="42"/>
+      <c r="J106" s="42" t="s">
         <v>331</v>
       </c>
-      <c r="H105" s="34" t="s">
-        <v>332</v>
-      </c>
-      <c r="I105" s="42"/>
-      <c r="J105" s="42" t="s">
-        <v>333</v>
-      </c>
-      <c r="K105" s="42"/>
-    </row>
-    <row r="106" spans="1:11" s="49" customFormat="1" ht="42">
-      <c r="A106" s="33"/>
-      <c r="B106" s="42" t="s">
-        <v>222</v>
-      </c>
-      <c r="C106" s="35"/>
-      <c r="D106" s="35"/>
-      <c r="E106" s="36"/>
-      <c r="F106" s="36"/>
-      <c r="G106" s="36"/>
-      <c r="H106" s="36"/>
-      <c r="I106" s="36" t="s">
-        <v>376</v>
-      </c>
-      <c r="J106" s="36" t="s">
-        <v>377</v>
-      </c>
-      <c r="K106" s="36"/>
-    </row>
-    <row r="107" spans="1:11" s="49" customFormat="1">
-      <c r="A107" s="15"/>
-      <c r="B107" s="15"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
-      <c r="G107" s="39"/>
-      <c r="H107" s="15"/>
-      <c r="I107" s="15"/>
-      <c r="J107" s="15"/>
-      <c r="K107" s="15"/>
-    </row>
-    <row r="108" spans="1:11">
+      <c r="K106" s="42"/>
+    </row>
+    <row r="107" spans="1:11" s="49" customFormat="1" ht="42">
+      <c r="A107" s="33"/>
+      <c r="B107" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="36"/>
+      <c r="F107" s="36"/>
+      <c r="G107" s="36"/>
+      <c r="H107" s="36"/>
+      <c r="I107" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="J107" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="K107" s="36"/>
+    </row>
+    <row r="108" spans="1:11" s="49" customFormat="1">
       <c r="A108" s="15"/>
       <c r="B108" s="15"/>
-      <c r="C108" s="16"/>
-      <c r="D108" s="16"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="15"/>
       <c r="E108" s="15"/>
       <c r="F108" s="15"/>
       <c r="G108" s="39"/>
@@ -7015,12 +7063,8 @@
       <c r="D109" s="16"/>
       <c r="E109" s="15"/>
       <c r="F109" s="15"/>
-      <c r="G109" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="H109" s="53" t="s">
-        <v>36</v>
-      </c>
+      <c r="G109" s="39"/>
+      <c r="H109" s="15"/>
       <c r="I109" s="15"/>
       <c r="J109" s="15"/>
       <c r="K109" s="15"/>
@@ -7032,11 +7076,11 @@
       <c r="D110" s="16"/>
       <c r="E110" s="15"/>
       <c r="F110" s="15"/>
-      <c r="G110" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="H110" s="31" t="s">
-        <v>38</v>
+      <c r="G110" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="H110" s="53" t="s">
+        <v>36</v>
       </c>
       <c r="I110" s="15"/>
       <c r="J110" s="15"/>
@@ -7049,11 +7093,11 @@
       <c r="D111" s="16"/>
       <c r="E111" s="15"/>
       <c r="F111" s="15"/>
-      <c r="G111" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="H111" s="15" t="s">
-        <v>39</v>
+      <c r="G111" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H111" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="I111" s="15"/>
       <c r="J111" s="15"/>
@@ -7067,10 +7111,10 @@
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
       <c r="G112" s="39" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
       <c r="H112" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I112" s="15"/>
       <c r="J112" s="15"/>
@@ -7084,10 +7128,10 @@
       <c r="E113" s="15"/>
       <c r="F113" s="15"/>
       <c r="G113" s="39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H113" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I113" s="15"/>
       <c r="J113" s="15"/>
@@ -7101,10 +7145,10 @@
       <c r="E114" s="15"/>
       <c r="F114" s="15"/>
       <c r="G114" s="39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H114" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I114" s="15"/>
       <c r="J114" s="15"/>
@@ -7118,10 +7162,10 @@
       <c r="E115" s="15"/>
       <c r="F115" s="15"/>
       <c r="G115" s="39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H115" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I115" s="15"/>
       <c r="J115" s="15"/>
@@ -7135,9 +7179,11 @@
       <c r="E116" s="15"/>
       <c r="F116" s="15"/>
       <c r="G116" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H116" s="15"/>
+        <v>46</v>
+      </c>
+      <c r="H116" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="I116" s="15"/>
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
@@ -7150,11 +7196,9 @@
       <c r="E117" s="15"/>
       <c r="F117" s="15"/>
       <c r="G117" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="H117" s="15" t="s">
-        <v>251</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="H117" s="15"/>
       <c r="I117" s="15"/>
       <c r="J117" s="15"/>
       <c r="K117" s="15"/>
@@ -7167,10 +7211,10 @@
       <c r="E118" s="15"/>
       <c r="F118" s="15"/>
       <c r="G118" s="39" t="s">
-        <v>49</v>
+        <v>249</v>
       </c>
       <c r="H118" s="15" t="s">
-        <v>113</v>
+        <v>250</v>
       </c>
       <c r="I118" s="15"/>
       <c r="J118" s="15"/>
@@ -7184,7 +7228,7 @@
       <c r="E119" s="15"/>
       <c r="F119" s="15"/>
       <c r="G119" s="39" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="H119" s="15" t="s">
         <v>112</v>
@@ -7201,10 +7245,10 @@
       <c r="E120" s="15"/>
       <c r="F120" s="15"/>
       <c r="G120" s="39" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="H120" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I120" s="15"/>
       <c r="J120" s="15"/>
@@ -7218,10 +7262,10 @@
       <c r="E121" s="15"/>
       <c r="F121" s="15"/>
       <c r="G121" s="39" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="H121" s="15" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="I121" s="15"/>
       <c r="J121" s="15"/>
@@ -7234,25 +7278,42 @@
       <c r="D122" s="16"/>
       <c r="E122" s="15"/>
       <c r="F122" s="15"/>
-      <c r="G122" s="39"/>
-      <c r="H122" s="15"/>
+      <c r="G122" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="H122" s="15" t="s">
+        <v>51</v>
+      </c>
       <c r="I122" s="15"/>
       <c r="J122" s="15"/>
       <c r="K122" s="15"/>
     </row>
     <row r="123" spans="1:11">
-      <c r="G123" s="39" t="s">
-        <v>114</v>
-      </c>
+      <c r="A123" s="15"/>
+      <c r="B123" s="15"/>
+      <c r="C123" s="16"/>
+      <c r="D123" s="16"/>
+      <c r="E123" s="15"/>
+      <c r="F123" s="15"/>
+      <c r="G123" s="39"/>
+      <c r="H123" s="15"/>
+      <c r="I123" s="15"/>
+      <c r="J123" s="15"/>
+      <c r="K123" s="15"/>
     </row>
     <row r="124" spans="1:11">
       <c r="G124" s="39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="125" spans="1:11">
       <c r="G125" s="39" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="G126" s="39" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to inventory and creation of folder for #1-6
</commit_message>
<xml_diff>
--- a/inventory/INVENTORY OF PYU INSCRIPTIONS.xlsx
+++ b/inventory/INVENTORY OF PYU INSCRIPTIONS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlogriffiths/Documents/git-repositories/pyu-inscriptions/inventory/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28380" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25540" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1380,9 +1385,6 @@
     <t>Middleton 2005: 173.</t>
   </si>
   <si>
-    <t>Middleton 2005, App.58</t>
-  </si>
-  <si>
     <t>Middleton's statement that the inscription is in Pali is incorrect.</t>
   </si>
   <si>
@@ -2881,13 +2883,16 @@
       </rPr>
       <t>—Tun Aung Chain 2003: 1-4.</t>
     </r>
+  </si>
+  <si>
+    <t>Middleton 2005, App.58, pp. 173-4.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3032,6 +3037,12 @@
       <sz val="12"/>
       <color rgb="FF0091CE"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3526,6 +3537,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3547,245 +3561,247 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="231">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -4074,13 +4090,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="5" bestFit="1" customWidth="1"/>
@@ -4092,7 +4111,7 @@
     <col min="11" max="11" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
@@ -4101,72 +4120,72 @@
       <c r="D1" s="4"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:11">
-      <c r="B2" s="63" t="s">
-        <v>373</v>
-      </c>
-      <c r="C2" s="63"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="64" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" s="64"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="64" t="s">
+      <c r="J3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="64" t="s">
+      <c r="K3" s="65" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="1:11" ht="59">
+      <c r="B4" s="66"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+    </row>
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C5" s="11">
         <v>2</v>
@@ -4187,14 +4206,14 @@
         <v>208</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="70">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -4218,16 +4237,16 @@
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="19" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="84">
+    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>3</v>
       </c>
@@ -4253,16 +4272,16 @@
         <v>6</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J7" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="56">
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>4</v>
       </c>
@@ -4288,14 +4307,14 @@
         <v>7</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="42">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>5</v>
       </c>
@@ -4321,14 +4340,14 @@
         <v>8</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" ht="70">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>6</v>
       </c>
@@ -4339,7 +4358,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>55</v>
@@ -4354,16 +4373,16 @@
         <v>9</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="84">
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -4389,16 +4408,16 @@
         <v>0</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="70">
+    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>8</v>
       </c>
@@ -4424,16 +4443,16 @@
         <v>247</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="42">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>9</v>
       </c>
@@ -4455,14 +4474,14 @@
         <v>22</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="42">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -4488,14 +4507,14 @@
         <v>22</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" ht="56">
+    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>11</v>
       </c>
@@ -4503,7 +4522,7 @@
         <v>81</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>241</v>
@@ -4521,16 +4540,16 @@
         <v>2</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="42">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -4557,13 +4576,13 @@
         <v>94</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="42">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="44">
         <v>13</v>
       </c>
@@ -4582,17 +4601,17 @@
         <v>220</v>
       </c>
       <c r="H17" s="62" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I17" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="J17" s="12" t="s">
-        <v>450</v>
-      </c>
       <c r="K17" s="46"/>
     </row>
-    <row r="18" spans="1:11" ht="266">
+    <row r="18" spans="1:11" ht="285" x14ac:dyDescent="0.2">
       <c r="A18" s="44">
         <v>14</v>
       </c>
@@ -4605,25 +4624,25 @@
       <c r="D18" s="30"/>
       <c r="E18" s="47"/>
       <c r="F18" s="46" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>220</v>
       </c>
       <c r="H18" s="45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I18" s="46" t="s">
+        <v>473</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="K18" s="46" t="s">
         <v>474</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="K18" s="46" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="42">
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="44">
         <v>15</v>
       </c>
@@ -4638,23 +4657,23 @@
         <v>55</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>220</v>
       </c>
       <c r="H19" s="46"/>
       <c r="I19" s="46" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K19" s="45" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="70">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>16</v>
       </c>
@@ -4665,13 +4684,13 @@
         <v>192</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>57</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G20" s="24" t="s">
         <v>160</v>
@@ -4681,11 +4700,11 @@
         <v>317</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" ht="42">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>17</v>
       </c>
@@ -4702,23 +4721,23 @@
         <v>55</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>194</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>324</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="22" customFormat="1" ht="56">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>18</v>
       </c>
@@ -4726,7 +4745,7 @@
         <v>79</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>236</v>
@@ -4735,7 +4754,7 @@
         <v>55</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>242</v>
@@ -4749,12 +4768,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="28">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C23" s="20">
         <v>3</v>
@@ -4780,7 +4799,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="22" customFormat="1" ht="70">
+    <row r="24" spans="1:11" s="22" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
         <v>20</v>
       </c>
@@ -4804,14 +4823,14 @@
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K24" s="13"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>21</v>
       </c>
@@ -4842,7 +4861,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="6" customFormat="1" ht="84">
+    <row r="26" spans="1:11" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
         <v>22</v>
       </c>
@@ -4866,16 +4885,16 @@
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="J26" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>462</v>
-      </c>
       <c r="K26" s="13" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="112">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>23</v>
       </c>
@@ -4897,7 +4916,7 @@
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>244</v>
@@ -4906,7 +4925,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="70">
+    <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>24</v>
       </c>
@@ -4923,26 +4942,26 @@
         <v>58</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>267</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K28" s="13"/>
     </row>
-    <row r="29" spans="1:11" ht="70">
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>25</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>28</v>
@@ -4964,13 +4983,13 @@
         <v>215</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="28">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
         <v>26</v>
       </c>
@@ -4987,23 +5006,23 @@
         <v>55</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>158</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="28">
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="21">
         <v>27</v>
       </c>
@@ -5027,14 +5046,14 @@
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" ht="42">
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" s="21">
         <v>28</v>
       </c>
@@ -5051,7 +5070,7 @@
         <v>55</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G32" s="24" t="s">
         <v>164</v>
@@ -5059,13 +5078,13 @@
       <c r="H32" s="13"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="28">
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="21">
         <v>29</v>
       </c>
@@ -5082,7 +5101,7 @@
         <v>55</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>165</v>
@@ -5093,15 +5112,15 @@
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="13" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="28">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="21">
         <v>30</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>29</v>
@@ -5113,7 +5132,7 @@
         <v>55</v>
       </c>
       <c r="F34" s="25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G34" s="24" t="s">
         <v>166</v>
@@ -5127,12 +5146,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="28">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
         <v>31</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>19</v>
@@ -5156,7 +5175,7 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
     </row>
-    <row r="36" spans="1:11" ht="42">
+    <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A36" s="21">
         <v>32</v>
       </c>
@@ -5173,23 +5192,23 @@
         <v>55</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13" t="s">
         <v>94</v>
       </c>
       <c r="J36" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="28">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="21">
         <v>33</v>
       </c>
@@ -5214,16 +5233,16 @@
         <v>205</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K37" s="13"/>
     </row>
-    <row r="38" spans="1:11" ht="42">
+    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A38" s="44">
         <v>34</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>19</v>
@@ -5242,16 +5261,16 @@
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>334</v>
+        <v>496</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>333</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="56">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="21">
         <v>35</v>
       </c>
@@ -5268,7 +5287,7 @@
         <v>55</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>200</v>
@@ -5282,73 +5301,73 @@
       </c>
       <c r="K39" s="13"/>
     </row>
-    <row r="40" spans="1:11" ht="56">
+    <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" s="44">
         <v>36</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>55</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="18" t="s">
         <v>94</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="84">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="90" x14ac:dyDescent="0.2">
       <c r="A41" s="21">
         <v>37</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>55</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="13" t="s">
         <v>94</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="22" customFormat="1" ht="28">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="21">
         <v>38</v>
       </c>
@@ -5379,7 +5398,7 @@
       </c>
       <c r="K42" s="13"/>
     </row>
-    <row r="43" spans="1:11" ht="42">
+    <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="21">
         <v>39</v>
       </c>
@@ -5393,7 +5412,7 @@
         <v>151</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F43" s="13" t="s">
         <v>105</v>
@@ -5410,7 +5429,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="56">
+    <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A44" s="21">
         <v>40</v>
       </c>
@@ -5434,16 +5453,16 @@
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="J44" s="13" t="s">
         <v>484</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>485</v>
       </c>
       <c r="K44" s="19" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="28">
+    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="21">
         <v>41</v>
       </c>
@@ -5474,7 +5493,7 @@
       </c>
       <c r="K45" s="13"/>
     </row>
-    <row r="46" spans="1:11" ht="42">
+    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A46" s="21">
         <v>42</v>
       </c>
@@ -5505,7 +5524,7 @@
       </c>
       <c r="K46" s="13"/>
     </row>
-    <row r="47" spans="1:11" ht="28">
+    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="21">
         <v>43</v>
       </c>
@@ -5525,19 +5544,19 @@
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K47" s="13"/>
     </row>
-    <row r="48" spans="1:11" ht="56">
+    <row r="48" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A48" s="21">
         <v>44</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>29</v>
@@ -5556,16 +5575,16 @@
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="J48" s="10" t="s">
         <v>486</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>487</v>
       </c>
       <c r="K48" s="13" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="42">
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>45</v>
       </c>
@@ -5573,30 +5592,30 @@
         <v>246</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>59</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="13" t="s">
         <v>270</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K49" s="13"/>
     </row>
-    <row r="50" spans="1:11" ht="56">
+    <row r="50" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>46</v>
       </c>
@@ -5614,7 +5633,7 @@
         <v>298</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="19" t="s">
@@ -5625,7 +5644,7 @@
       </c>
       <c r="K50" s="13"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="56">
         <v>47</v>
       </c>
@@ -5643,16 +5662,16 @@
         <v>108</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H51" s="18"/>
       <c r="I51" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="18"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="56">
         <v>48</v>
       </c>
@@ -5670,16 +5689,16 @@
         <v>108</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H52" s="18"/>
       <c r="I52" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="18"/>
     </row>
-    <row r="53" spans="1:11" ht="28">
+    <row r="53" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="21">
         <v>49</v>
       </c>
@@ -5704,11 +5723,11 @@
         <v>222</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K53" s="19"/>
     </row>
-    <row r="54" spans="1:11" ht="28">
+    <row r="54" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="44">
         <v>50</v>
       </c>
@@ -5737,7 +5756,7 @@
       </c>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="1:11" ht="28">
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="21">
         <v>51</v>
       </c>
@@ -5766,7 +5785,7 @@
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
     </row>
-    <row r="56" spans="1:11" ht="28">
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="21">
         <v>52</v>
       </c>
@@ -5790,14 +5809,14 @@
       </c>
       <c r="H56" s="19"/>
       <c r="I56" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J56" s="19" t="s">
         <v>74</v>
       </c>
       <c r="K56" s="19"/>
     </row>
-    <row r="57" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="57" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="21">
         <v>53</v>
       </c>
@@ -5821,14 +5840,14 @@
       </c>
       <c r="H57" s="19"/>
       <c r="I57" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J57" s="19" t="s">
         <v>74</v>
       </c>
       <c r="K57" s="19"/>
     </row>
-    <row r="58" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="58" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="21">
         <v>54</v>
       </c>
@@ -5852,14 +5871,14 @@
       </c>
       <c r="H58" s="19"/>
       <c r="I58" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J58" s="19" t="s">
         <v>74</v>
       </c>
       <c r="K58" s="19"/>
     </row>
-    <row r="59" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="59" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="21">
         <v>55</v>
       </c>
@@ -5884,7 +5903,7 @@
       </c>
       <c r="K59" s="19"/>
     </row>
-    <row r="60" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="60" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="21">
         <v>56</v>
       </c>
@@ -5907,7 +5926,7 @@
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
     </row>
-    <row r="61" spans="1:11" s="22" customFormat="1" ht="42">
+    <row r="61" spans="1:11" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A61" s="21">
         <v>57</v>
       </c>
@@ -5930,7 +5949,7 @@
       <c r="J61" s="19"/>
       <c r="K61" s="19"/>
     </row>
-    <row r="62" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="62" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="44">
         <v>58</v>
       </c>
@@ -5961,41 +5980,41 @@
       </c>
       <c r="K62" s="23"/>
     </row>
-    <row r="63" spans="1:11" s="22" customFormat="1" ht="56">
+    <row r="63" spans="1:11" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A63" s="21">
         <v>59</v>
       </c>
       <c r="B63" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="C63" s="20" t="s">
         <v>359</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>360</v>
       </c>
       <c r="D63" s="20"/>
       <c r="E63" s="19" t="s">
         <v>107</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G63" s="23" t="s">
         <v>108</v>
       </c>
       <c r="H63" s="23"/>
       <c r="I63" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J63" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K63" s="19"/>
     </row>
-    <row r="64" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="64" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" s="21">
         <v>60</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>19</v>
@@ -6017,7 +6036,7 @@
       <c r="J64" s="19"/>
       <c r="K64" s="19"/>
     </row>
-    <row r="65" spans="1:11" s="22" customFormat="1" ht="56">
+    <row r="65" spans="1:11" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A65" s="21">
         <v>61</v>
       </c>
@@ -6034,7 +6053,7 @@
         <v>55</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G65" s="23" t="s">
         <v>184</v>
@@ -6048,7 +6067,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="22" customFormat="1">
+    <row r="66" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44">
         <v>62</v>
       </c>
@@ -6068,12 +6087,12 @@
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J66" s="12"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="67" spans="1:11" s="50" customFormat="1" ht="42">
+    <row r="67" spans="1:11" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A67" s="44">
         <v>63</v>
       </c>
@@ -6084,29 +6103,29 @@
         <v>19</v>
       </c>
       <c r="D67" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="G67" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="H67" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="I67" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="F67" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="H67" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="I67" s="12" t="s">
+      <c r="J67" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="J67" s="12" t="s">
-        <v>383</v>
-      </c>
       <c r="K67" s="12"/>
     </row>
-    <row r="68" spans="1:11" s="22" customFormat="1" ht="70">
+    <row r="68" spans="1:11" s="22" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A68" s="44">
         <v>64</v>
       </c>
@@ -6121,17 +6140,17 @@
         <v>55</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
       <c r="K68" s="12" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="22" customFormat="1" ht="42">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="44">
         <v>65</v>
       </c>
@@ -6146,23 +6165,23 @@
         <v>55</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G69" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="J69" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="H69" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="I69" s="12" t="s">
-        <v>389</v>
-      </c>
-      <c r="J69" s="12" t="s">
-        <v>397</v>
-      </c>
       <c r="K69" s="12"/>
     </row>
-    <row r="70" spans="1:11" s="60" customFormat="1" ht="42">
+    <row r="70" spans="1:11" s="60" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A70" s="57">
         <v>66</v>
       </c>
@@ -6177,23 +6196,23 @@
         <v>55</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G70" s="25" t="s">
         <v>108</v>
       </c>
       <c r="H70" s="59" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J70" s="24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K70" s="59"/>
     </row>
-    <row r="71" spans="1:11" s="49" customFormat="1" ht="42">
+    <row r="71" spans="1:11" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A71" s="44">
         <v>67</v>
       </c>
@@ -6204,7 +6223,7 @@
         <v>103</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>55</v>
@@ -6213,19 +6232,19 @@
         <v>108</v>
       </c>
       <c r="G71" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J71" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K71" s="18"/>
     </row>
-    <row r="72" spans="1:11" s="49" customFormat="1">
-      <c r="A72" s="70">
+    <row r="72" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="63">
         <v>68</v>
       </c>
       <c r="B72" s="36" t="s">
@@ -6241,12 +6260,12 @@
       <c r="H72" s="36"/>
       <c r="I72" s="36"/>
       <c r="J72" s="36" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K72" s="36"/>
     </row>
-    <row r="73" spans="1:11" s="49" customFormat="1">
-      <c r="A73" s="70">
+    <row r="73" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="63">
         <v>69</v>
       </c>
       <c r="B73" s="36" t="s">
@@ -6262,12 +6281,12 @@
       <c r="H73" s="36"/>
       <c r="I73" s="36"/>
       <c r="J73" s="36" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K73" s="36"/>
     </row>
-    <row r="74" spans="1:11" s="22" customFormat="1" ht="28">
-      <c r="A74" s="70">
+    <row r="74" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A74" s="63">
         <v>70</v>
       </c>
       <c r="B74" s="42" t="s">
@@ -6289,11 +6308,11 @@
         <v>311</v>
       </c>
       <c r="J74" s="42" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K74" s="42"/>
     </row>
-    <row r="75" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="75" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="41"/>
       <c r="B75" s="42" t="s">
         <v>106</v>
@@ -6309,14 +6328,14 @@
       </c>
       <c r="H75" s="42"/>
       <c r="I75" s="61" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J75" s="42" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K75" s="42"/>
     </row>
-    <row r="76" spans="1:11" s="22" customFormat="1">
+    <row r="76" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="41"/>
       <c r="B76" s="42" t="s">
         <v>280</v>
@@ -6341,7 +6360,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="77" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="41"/>
       <c r="B77" s="42" t="s">
         <v>280</v>
@@ -6368,7 +6387,7 @@
       </c>
       <c r="K77" s="36"/>
     </row>
-    <row r="78" spans="1:11" s="22" customFormat="1" ht="56">
+    <row r="78" spans="1:11" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A78" s="41"/>
       <c r="B78" s="42" t="s">
         <v>106</v>
@@ -6381,23 +6400,23 @@
         <v>55</v>
       </c>
       <c r="F78" s="42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G78" s="42" t="s">
         <v>108</v>
       </c>
       <c r="H78" s="42"/>
       <c r="I78" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="J78" s="42" t="s">
+        <v>343</v>
+      </c>
+      <c r="K78" s="42" t="s">
         <v>342</v>
       </c>
-      <c r="J78" s="42" t="s">
-        <v>344</v>
-      </c>
-      <c r="K78" s="42" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="22" customFormat="1" ht="28">
+    </row>
+    <row r="79" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="41"/>
       <c r="B79" s="42" t="s">
         <v>106</v>
@@ -6420,7 +6439,7 @@
       </c>
       <c r="K79" s="42"/>
     </row>
-    <row r="80" spans="1:11" s="22" customFormat="1">
+    <row r="80" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="41"/>
       <c r="B80" s="42" t="s">
         <v>106</v>
@@ -6439,7 +6458,7 @@
       </c>
       <c r="K80" s="42"/>
     </row>
-    <row r="81" spans="1:11" s="22" customFormat="1" ht="112">
+    <row r="81" spans="1:11" s="22" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A81" s="54"/>
       <c r="B81" s="37" t="s">
         <v>106</v>
@@ -6468,7 +6487,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="82" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="41"/>
       <c r="B82" s="42" t="s">
         <v>106</v>
@@ -6491,7 +6510,7 @@
       </c>
       <c r="K82" s="42"/>
     </row>
-    <row r="83" spans="1:11" s="22" customFormat="1">
+    <row r="83" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="41"/>
       <c r="B83" s="42" t="s">
         <v>106</v>
@@ -6516,7 +6535,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="84" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" s="41"/>
       <c r="B84" s="42" t="s">
         <v>106</v>
@@ -6541,7 +6560,7 @@
       </c>
       <c r="K84" s="42"/>
     </row>
-    <row r="85" spans="1:11" s="22" customFormat="1">
+    <row r="85" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="41"/>
       <c r="B85" s="42" t="s">
         <v>106</v>
@@ -6560,7 +6579,7 @@
       </c>
       <c r="K85" s="42"/>
     </row>
-    <row r="86" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="86" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" s="41"/>
       <c r="B86" s="42" t="s">
         <v>106</v>
@@ -6581,7 +6600,7 @@
       </c>
       <c r="K86" s="42"/>
     </row>
-    <row r="88" spans="1:11" s="22" customFormat="1">
+    <row r="88" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="41"/>
       <c r="B88" s="42" t="s">
         <v>280</v>
@@ -6606,30 +6625,30 @@
       </c>
       <c r="K88" s="42"/>
     </row>
-    <row r="89" spans="1:11" s="22" customFormat="1" ht="28">
+    <row r="89" spans="1:11" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="41"/>
       <c r="B89" s="42" t="s">
         <v>280</v>
       </c>
       <c r="C89" s="43" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D89" s="43"/>
       <c r="E89" s="34" t="s">
         <v>55</v>
       </c>
       <c r="F89" s="42" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G89" s="34"/>
       <c r="H89" s="42"/>
       <c r="I89" s="42"/>
       <c r="J89" s="42" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K89" s="42"/>
     </row>
-    <row r="90" spans="1:11" s="22" customFormat="1">
+    <row r="90" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="33"/>
       <c r="B90" s="34" t="s">
         <v>106</v>
@@ -6648,7 +6667,7 @@
       <c r="J90" s="36"/>
       <c r="K90" s="36"/>
     </row>
-    <row r="91" spans="1:11" s="22" customFormat="1">
+    <row r="91" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="33"/>
       <c r="B91" s="34" t="s">
         <v>106</v>
@@ -6667,7 +6686,7 @@
       <c r="J91" s="36"/>
       <c r="K91" s="36"/>
     </row>
-    <row r="92" spans="1:11" ht="42">
+    <row r="92" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A92" s="33"/>
       <c r="B92" s="34" t="s">
         <v>32</v>
@@ -6686,24 +6705,24 @@
       </c>
       <c r="K92" s="36"/>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="33"/>
       <c r="B93" s="34"/>
       <c r="C93" s="35"/>
       <c r="D93" s="35"/>
       <c r="E93" s="36"/>
       <c r="F93" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G93" s="36"/>
       <c r="H93" s="36"/>
       <c r="I93" s="36"/>
       <c r="J93" s="36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K93" s="36"/>
     </row>
-    <row r="94" spans="1:11" ht="28">
+    <row r="94" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="41"/>
       <c r="B94" s="42" t="s">
         <v>52</v>
@@ -6715,16 +6734,16 @@
       <c r="E94" s="34"/>
       <c r="F94" s="42"/>
       <c r="G94" s="42" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H94" s="42"/>
       <c r="I94" s="42"/>
       <c r="J94" s="42"/>
       <c r="K94" s="42" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" s="50" customFormat="1" ht="98">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" s="50" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A95" s="41"/>
       <c r="B95" s="42" t="s">
         <v>52</v>
@@ -6751,7 +6770,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="49" customFormat="1">
+    <row r="96" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="41"/>
       <c r="B96" s="42" t="s">
         <v>63</v>
@@ -6774,7 +6793,7 @@
       </c>
       <c r="K96" s="42"/>
     </row>
-    <row r="97" spans="1:11" s="50" customFormat="1">
+    <row r="97" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="41"/>
       <c r="B97" s="42" t="s">
         <v>63</v>
@@ -6797,7 +6816,7 @@
       </c>
       <c r="K97" s="42"/>
     </row>
-    <row r="98" spans="1:11" s="50" customFormat="1">
+    <row r="98" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="41"/>
       <c r="B98" s="42" t="s">
         <v>63</v>
@@ -6820,7 +6839,7 @@
       </c>
       <c r="K98" s="42"/>
     </row>
-    <row r="99" spans="1:11" s="50" customFormat="1">
+    <row r="99" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="41"/>
       <c r="B99" s="42" t="s">
         <v>65</v>
@@ -6845,7 +6864,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="50" customFormat="1">
+    <row r="100" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="41"/>
       <c r="B100" s="42" t="s">
         <v>233</v>
@@ -6870,7 +6889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="50" customFormat="1" ht="28">
+    <row r="101" spans="1:11" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="41"/>
       <c r="B101" s="42" t="s">
         <v>72</v>
@@ -6899,7 +6918,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="50" customFormat="1" ht="28">
+    <row r="102" spans="1:11" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A102" s="41"/>
       <c r="B102" s="42" t="s">
         <v>235</v>
@@ -6920,11 +6939,11 @@
       </c>
       <c r="I102" s="42"/>
       <c r="J102" s="42" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K102" s="42"/>
     </row>
-    <row r="103" spans="1:11" s="50" customFormat="1" ht="28">
+    <row r="103" spans="1:11" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A103" s="41"/>
       <c r="B103" s="42" t="s">
         <v>327</v>
@@ -6945,11 +6964,11 @@
       </c>
       <c r="I103" s="42"/>
       <c r="J103" s="42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K103" s="42"/>
     </row>
-    <row r="104" spans="1:11" s="50" customFormat="1" ht="28">
+    <row r="104" spans="1:11" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A104" s="41"/>
       <c r="B104" s="42" t="s">
         <v>326</v>
@@ -6970,13 +6989,13 @@
       </c>
       <c r="I104" s="42"/>
       <c r="J104" s="42" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K104" s="42" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" s="50" customFormat="1" ht="182">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" s="50" customFormat="1" ht="195" x14ac:dyDescent="0.2">
       <c r="A105" s="41"/>
       <c r="B105" s="42" t="s">
         <v>183</v>
@@ -6996,16 +7015,16 @@
         <v>185</v>
       </c>
       <c r="I105" s="42" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J105" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K105" s="42" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" s="50" customFormat="1">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="41"/>
       <c r="B106" s="42"/>
       <c r="C106" s="43"/>
@@ -7024,7 +7043,7 @@
       </c>
       <c r="K106" s="42"/>
     </row>
-    <row r="107" spans="1:11" s="49" customFormat="1" ht="42">
+    <row r="107" spans="1:11" s="49" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A107" s="33"/>
       <c r="B107" s="42" t="s">
         <v>221</v>
@@ -7036,14 +7055,14 @@
       <c r="G107" s="36"/>
       <c r="H107" s="36"/>
       <c r="I107" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="J107" s="36" t="s">
         <v>374</v>
       </c>
-      <c r="J107" s="36" t="s">
-        <v>375</v>
-      </c>
       <c r="K107" s="36"/>
     </row>
-    <row r="108" spans="1:11" s="49" customFormat="1">
+    <row r="108" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
@@ -7056,7 +7075,7 @@
       <c r="J108" s="15"/>
       <c r="K108" s="15"/>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
       <c r="C109" s="16"/>
@@ -7069,7 +7088,7 @@
       <c r="J109" s="15"/>
       <c r="K109" s="15"/>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="15"/>
       <c r="B110" s="15"/>
       <c r="C110" s="16"/>
@@ -7086,7 +7105,7 @@
       <c r="J110" s="15"/>
       <c r="K110" s="15"/>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="15"/>
       <c r="B111" s="15"/>
       <c r="C111" s="16"/>
@@ -7103,7 +7122,7 @@
       <c r="J111" s="15"/>
       <c r="K111" s="15"/>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="15"/>
       <c r="B112" s="15"/>
       <c r="C112" s="16"/>
@@ -7120,7 +7139,7 @@
       <c r="J112" s="15"/>
       <c r="K112" s="15"/>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="15"/>
       <c r="B113" s="15"/>
       <c r="C113" s="16"/>
@@ -7137,7 +7156,7 @@
       <c r="J113" s="15"/>
       <c r="K113" s="15"/>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="15"/>
       <c r="B114" s="15"/>
       <c r="C114" s="16"/>
@@ -7154,7 +7173,7 @@
       <c r="J114" s="15"/>
       <c r="K114" s="15"/>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="15"/>
       <c r="B115" s="15"/>
       <c r="C115" s="16"/>
@@ -7171,7 +7190,7 @@
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="15"/>
       <c r="B116" s="15"/>
       <c r="C116" s="16"/>
@@ -7188,7 +7207,7 @@
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="15"/>
       <c r="B117" s="15"/>
       <c r="C117" s="16"/>
@@ -7203,7 +7222,7 @@
       <c r="J117" s="15"/>
       <c r="K117" s="15"/>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="15"/>
       <c r="B118" s="15"/>
       <c r="C118" s="16"/>
@@ -7220,7 +7239,7 @@
       <c r="J118" s="15"/>
       <c r="K118" s="15"/>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="15"/>
       <c r="B119" s="15"/>
       <c r="C119" s="16"/>
@@ -7237,7 +7256,7 @@
       <c r="J119" s="15"/>
       <c r="K119" s="15"/>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="15"/>
       <c r="B120" s="15"/>
       <c r="C120" s="16"/>
@@ -7254,7 +7273,7 @@
       <c r="J120" s="15"/>
       <c r="K120" s="15"/>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="15"/>
       <c r="B121" s="15"/>
       <c r="C121" s="16"/>
@@ -7271,7 +7290,7 @@
       <c r="J121" s="15"/>
       <c r="K121" s="15"/>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="15"/>
       <c r="B122" s="15"/>
       <c r="C122" s="16"/>
@@ -7288,7 +7307,7 @@
       <c r="J122" s="15"/>
       <c r="K122" s="15"/>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="15"/>
       <c r="B123" s="15"/>
       <c r="C123" s="16"/>
@@ -7301,17 +7320,17 @@
       <c r="J123" s="15"/>
       <c r="K123" s="15"/>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G124" s="39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G125" s="39" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G126" s="39" t="s">
         <v>125</v>
       </c>
@@ -7332,12 +7351,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" scale="14" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
@@ -7347,14 +7361,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7364,13 +7375,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>